<commit_message>
Added magnets, assembly is so slow now.
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02be13960f358456/projects/splitFlapDisplay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawai\OneDrive\projects\splitFlapDisplay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Feature</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>beltLength</t>
+  </si>
+  <si>
+    <t>magnetDiameter</t>
+  </si>
+  <si>
+    <t>magnetLength</t>
+  </si>
+  <si>
+    <t>magnetProtusion</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,6 +712,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>0.25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Electroincs setup proerly, ready for build... i think
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawai\OneDrive\projects\splitFlapDisplay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\splitFlapDisplay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Feature</t>
   </si>
@@ -120,12 +120,18 @@
   </si>
   <si>
     <t>magnetProtusion</t>
+  </si>
+  <si>
+    <t>notchWidth</t>
+  </si>
+  <si>
+    <t>spoolThickness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,6 +256,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -285,6 +308,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +526,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -497,7 +537,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -706,7 +746,7 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>350</v>
+        <v>240</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -728,7 +768,7 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -743,6 +783,28 @@
       </c>
       <c r="C27" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>0.22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pattrens changed size so it fits
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -480,7 +480,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +559,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Wrote makefile, included renders, removed showcase, blender
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\splitFlapDisplay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\splitFlapDisplay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -480,12 +480,12 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>

</xml_diff>